<commit_message>
Updated business plan & Risk assessment documents
</commit_message>
<xml_diff>
--- a/docs/Deliverable2-Risk Assessment.xlsx
+++ b/docs/Deliverable2-Risk Assessment.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25825"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,10 +15,21 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -27,128 +38,128 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
+    <t>RiskID</t>
+  </si>
+  <si>
     <t>Risk</t>
   </si>
   <si>
+    <t>Probability Description</t>
+  </si>
+  <si>
     <t>Probability</t>
   </si>
   <si>
+    <t>Effect Description</t>
+  </si>
+  <si>
     <t>Effect</t>
   </si>
   <si>
+    <t>Our Plan</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>The time required to develop the software is underestimated</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Serious</t>
+  </si>
+  <si>
+    <t>Reschedule the whole project, hire more developers or divide the project by phases</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
     <t>Cloud service is unavailable or underperformance</t>
   </si>
   <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>Look for another cloud service</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
     <t>API service is unavailable</t>
   </si>
   <si>
+    <t>Tolerable</t>
+  </si>
+  <si>
+    <t>Price Comparison function may need to disable until the API service is resumed</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
     <t>Change in management (requiring fewer developers)</t>
   </si>
   <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Reallocated tasks of the developers</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
     <t>Lack of developers due to virus outbreak</t>
   </si>
   <si>
+    <t>May need to reschedule the whole project</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
     <t>Client changes all the requirement</t>
   </si>
   <si>
+    <t>May need to seize the project and plan a new one</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
     <t>Scope of projects on payment gateway integration is underestimated</t>
   </si>
   <si>
+    <t>Hire payment gateway experts</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
     <t>Software tools no longer supported</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Moderate</t>
-  </si>
-  <si>
-    <t>The time required to develop the software is underestimated</t>
-  </si>
-  <si>
-    <t>Serious</t>
-  </si>
-  <si>
-    <t>Our Plan</t>
-  </si>
-  <si>
-    <t>Tolerable</t>
+    <t>Search new software tools</t>
+  </si>
+  <si>
+    <t>R9</t>
   </si>
   <si>
     <t>Legal issues on copyrights (e.g. on product images)</t>
   </si>
   <si>
-    <t>May need to reschedule the whole project</t>
-  </si>
-  <si>
-    <t>Price Comparison function may need to disable until the API service is resumed</t>
-  </si>
-  <si>
-    <t>May need to seize the project and plan a new one</t>
-  </si>
-  <si>
-    <t>Hire payment gateway experts</t>
-  </si>
-  <si>
-    <t>Reschedule the whole project, hire more developers or divide the project by phases</t>
-  </si>
-  <si>
-    <t>Look for another cloud service</t>
-  </si>
-  <si>
-    <t>Reallocated tasks of the developers</t>
-  </si>
-  <si>
-    <t>Search new software tools</t>
-  </si>
-  <si>
     <t>Take the project images by ourselves</t>
-  </si>
-  <si>
-    <t>RiskID</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>Effect Description</t>
-  </si>
-  <si>
-    <t>Probability Description</t>
-  </si>
-  <si>
-    <t>Low</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,10 +211,10 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1648,10 +1659,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{192616D0-D03E-42AD-8BD5-025648860050}" name="Table1" displayName="Table1" ref="A1:G10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G10" xr:uid="{192616D0-D03E-42AD-8BD5-025648860050}"/>
@@ -1661,8 +1668,8 @@
     <tableColumn id="2" xr3:uid="{4CF717F6-268E-445E-98F1-C60DCE6C077C}" name="Probability Description" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{21BF3997-6316-429F-A78B-8C90DC91EB72}" name="Probability" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{B88224A8-D779-4507-A263-3FDC1AAB1DD1}" name="Effect Description" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{0D574DEC-8A22-40C8-A4B5-5D7211EF5502}" name="Effect" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{16BF9B67-B6C5-4E62-A737-43547AB97C77}" name="Our Plan" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{0D574DEC-8A22-40C8-A4B5-5D7211EF5502}" name="Effect" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{16BF9B67-B6C5-4E62-A737-43547AB97C77}" name="Our Plan" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1937,125 +1944,125 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="14.65"/>
   <cols>
-    <col min="1" max="1" width="8.15234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.4609375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.07421875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.4609375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="70.3828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.23046875" style="2"/>
+    <col min="1" max="1" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="70.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="29.1">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="29.1">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3">
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3">
         <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3">
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3">
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F5" s="3">
         <v>5</v>
@@ -2064,119 +2071,119 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3">
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3">
         <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3">
         <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="3">
         <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F8" s="3">
         <v>7</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3">
         <v>3</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F9" s="3">
         <v>6</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3">
         <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F10" s="3">
         <v>4</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>